<commit_message>
diagramas y requisitos actualizados
</commit_message>
<xml_diff>
--- a/entornos-desarrollo/Casos de uso/CasosDeUso.xlsx
+++ b/entornos-desarrollo/Casos de uso/CasosDeUso.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31d722e80a21f9fd/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiach\Desktop\DAM\PracticaGrupalITV\Proyecto_Grupal-ITV\entornos-desarrollo\Casos de uso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70B224E4-18A9-45BE-99EB-EB8113F9FA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5E2B55-F834-4FBA-B5DE-FC44FBF49C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F41F7156-858F-464E-AF25-50B6BA6BE90F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{F41F7156-858F-464E-AF25-50B6BA6BE90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="112">
   <si>
     <t>Código:</t>
   </si>
@@ -74,9 +74,6 @@
     <t>se habrá mostrado el error que se haya producido.</t>
   </si>
   <si>
-    <t>si no es exitoso, se habrá mostrado el error que se haya producido.</t>
-  </si>
-  <si>
     <t>borrarVehiculo</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>CU-06</t>
   </si>
   <si>
-    <t>Si el proceso fue exitoso, se añadirá un nuevo vehículo en la BBDD, si no es exitoso,</t>
-  </si>
-  <si>
     <t xml:space="preserve">Si el proceso fue exitoso, se habrán aplicado cambios al vehículo seleccionado en la BBDD, </t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>y haber seleccionado la opcion de "añadir propietario"</t>
   </si>
   <si>
-    <t>Si el proceso fue exitoso, se añadirá un nuevo propieatrio en la BBDD, si no es exitoso,</t>
-  </si>
-  <si>
     <t>2.1. Si se selecciona "aceptar", se trata de crear el propietario, si algo falla, no se crea y se devuelve el error.</t>
   </si>
   <si>
@@ -233,9 +224,6 @@
     <t>Haber iniciado el programa, haber seleccionado previemente la opción de "añadir informe".</t>
   </si>
   <si>
-    <t>Si el proceso fue exitoso, se añadirá un nuevo informe en la BBDD, si no es exitoso,</t>
-  </si>
-  <si>
     <t>1. Rellenar los campos del informe a crear (como mínimo los que hacen a una cita).</t>
   </si>
   <si>
@@ -305,9 +293,6 @@
     <t>RF-33;crear un nuevo trabajador.</t>
   </si>
   <si>
-    <t>Si el proceso fue exitoso, se habrá añadido el nuevo trabajador en la BBDD, si no es exitoso,</t>
-  </si>
-  <si>
     <t>se habrá mostrado el error ocurrido.</t>
   </si>
   <si>
@@ -347,12 +332,6 @@
     <t>1.1. Si se selecciona "aceptar", se trata de eliminar el trabajador, si algo falla, no se elimina y se devuelve el error.</t>
   </si>
   <si>
-    <t>Falta la inspección de vehículos, mirar el enuncuado</t>
-  </si>
-  <si>
-    <t>También falta que alguién haga el Diagram de Clases</t>
-  </si>
-  <si>
     <t>CU-13</t>
   </si>
   <si>
@@ -371,21 +350,44 @@
     <t>"iniciar inspeccion"</t>
   </si>
   <si>
-    <t>seleccionada, ademas de actualizarse la cita , si no es exitoso, se habrá mostrado el error ocurrido.</t>
-  </si>
-  <si>
     <t>1. Seleccionar la opción "aceptar" o "cancelar".</t>
   </si>
   <si>
     <t>1.1. Si se selecciona "aceptar", se trata de actualizar la cita, si algo falla, no se actualiza y se devuelve el error.</t>
+  </si>
+  <si>
+    <t>Si el proceso fue exitoso, se añadirá un nuevo vehículo en la BBDD, si no fue exitoso,</t>
+  </si>
+  <si>
+    <t>si no fue exitoso, se habrá mostrado el error que se haya producido.</t>
+  </si>
+  <si>
+    <t>Si el proceso fue exitoso, se añadirá un nuevo propieatrio en la BBDD, si no fue exitoso,</t>
+  </si>
+  <si>
+    <t>Si el proceso fue exitoso, se añadirá un nuevo informe en la BBDD, si no fue exitoso,</t>
+  </si>
+  <si>
+    <t>Si el proceso fue exitoso, se habrá añadido el nuevo trabajador en la BBDD, si no fue exitoso,</t>
+  </si>
+  <si>
+    <t>seleccionada, ademas de actualizarse la cita , si no fue exitoso, se habrá mostrado el error ocurrido.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -544,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -568,6 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DDF1A6-7382-480A-BCCE-FA73B25350DD}">
-  <dimension ref="A2:I285"/>
+  <dimension ref="A2:O285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="H267" sqref="H267"/>
+    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="142" workbookViewId="0">
+      <selection activeCell="L235" sqref="L235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +899,7 @@
     <col min="6" max="6" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -905,13 +908,13 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="10" t="s">
@@ -922,7 +925,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -930,11 +933,8 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="6"/>
-      <c r="I4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
@@ -950,11 +950,8 @@
         <v>8</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="I5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -963,7 +960,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="12" t="s">
         <v>4</v>
@@ -974,10 +971,10 @@
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -985,10 +982,10 @@
       <c r="F8" s="3"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -996,7 +993,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1005,7 +1002,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="12" t="s">
         <v>5</v>
@@ -1016,10 +1013,10 @@
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1027,7 +1024,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
         <v>11</v>
@@ -1038,7 +1035,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1047,10 +1044,10 @@
       <c r="F14" s="5"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1058,10 +1055,10 @@
       <c r="F15" s="15"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -1072,7 +1069,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1083,7 +1080,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -1094,7 +1091,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1105,7 +1102,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -1137,7 +1134,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="10" t="s">
@@ -1197,7 +1194,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1208,7 +1205,7 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1239,7 +1236,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1250,7 +1247,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1270,7 +1267,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -1281,7 +1278,7 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -1292,7 +1289,7 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
@@ -1303,7 +1300,7 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -1314,7 +1311,7 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -1325,7 +1322,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -1357,14 +1354,14 @@
         <v>0</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G47" s="6"/>
     </row>
@@ -1383,7 +1380,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D49" s="5"/>
       <c r="E49" s="10" t="s">
@@ -1417,7 +1414,7 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1428,7 +1425,7 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -1459,7 +1456,7 @@
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -1470,7 +1467,7 @@
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -1490,7 +1487,7 @@
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
@@ -1501,7 +1498,7 @@
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -1512,7 +1509,7 @@
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
@@ -1523,7 +1520,7 @@
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
@@ -1534,7 +1531,7 @@
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -1575,14 +1572,14 @@
         <v>0</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G69" s="6"/>
     </row>
@@ -1601,7 +1598,7 @@
         <v>2</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="10" t="s">
@@ -1635,7 +1632,7 @@
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -1646,7 +1643,7 @@
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
@@ -1677,7 +1674,7 @@
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="1" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
@@ -1708,7 +1705,7 @@
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
@@ -1719,7 +1716,7 @@
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="18"/>
@@ -1730,7 +1727,7 @@
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
@@ -1741,7 +1738,7 @@
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="15"/>
@@ -1752,7 +1749,7 @@
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="15"/>
@@ -1763,7 +1760,7 @@
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C86" s="21"/>
       <c r="D86" s="21"/>
@@ -1795,14 +1792,14 @@
         <v>0</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G91" s="6"/>
     </row>
@@ -1821,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="10" t="s">
@@ -1855,7 +1852,7 @@
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -1866,7 +1863,7 @@
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
@@ -1897,7 +1894,7 @@
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -1908,7 +1905,7 @@
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
@@ -1928,7 +1925,7 @@
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
       <c r="B103" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C103" s="15"/>
       <c r="D103" s="15"/>
@@ -1939,7 +1936,7 @@
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
       <c r="B104" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C104" s="18"/>
       <c r="D104" s="18"/>
@@ -1950,7 +1947,7 @@
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="13"/>
       <c r="B105" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C105" s="15"/>
       <c r="D105" s="15"/>
@@ -1961,7 +1958,7 @@
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="13"/>
       <c r="B106" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C106" s="15"/>
       <c r="D106" s="15"/>
@@ -1972,7 +1969,7 @@
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
       <c r="B107" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C107" s="15"/>
       <c r="D107" s="15"/>
@@ -1983,7 +1980,7 @@
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="13"/>
       <c r="B108" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C108" s="21"/>
       <c r="D108" s="21"/>
@@ -2015,14 +2012,14 @@
         <v>0</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D113" s="5"/>
       <c r="E113" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G113" s="6"/>
     </row>
@@ -2041,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D115" s="5"/>
       <c r="E115" s="10" t="s">
@@ -2075,7 +2072,7 @@
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -2086,7 +2083,7 @@
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
@@ -2117,7 +2114,7 @@
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
@@ -2128,7 +2125,7 @@
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
@@ -2148,7 +2145,7 @@
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
       <c r="B125" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C125" s="15"/>
       <c r="D125" s="15"/>
@@ -2159,7 +2156,7 @@
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
       <c r="B126" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C126" s="18"/>
       <c r="D126" s="18"/>
@@ -2170,7 +2167,7 @@
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="15"/>
@@ -2181,7 +2178,7 @@
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
       <c r="B128" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C128" s="15"/>
       <c r="D128" s="15"/>
@@ -2192,7 +2189,7 @@
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
       <c r="B129" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C129" s="15"/>
       <c r="D129" s="15"/>
@@ -2233,14 +2230,14 @@
         <v>0</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D135" s="5"/>
       <c r="E135" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G135" s="6"/>
     </row>
@@ -2259,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D137" s="5"/>
       <c r="E137" s="10" t="s">
@@ -2293,7 +2290,7 @@
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
@@ -2333,7 +2330,7 @@
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="1" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
@@ -2364,7 +2361,7 @@
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="13"/>
       <c r="B147" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C147" s="15"/>
       <c r="D147" s="15"/>
@@ -2375,7 +2372,7 @@
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="13"/>
       <c r="B148" s="17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C148" s="18"/>
       <c r="D148" s="18"/>
@@ -2386,7 +2383,7 @@
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
       <c r="B149" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C149" s="15"/>
       <c r="D149" s="15"/>
@@ -2397,7 +2394,7 @@
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="13"/>
       <c r="B150" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C150" s="15"/>
       <c r="D150" s="15"/>
@@ -2408,7 +2405,7 @@
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="13"/>
       <c r="B151" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C151" s="15"/>
       <c r="D151" s="15"/>
@@ -2419,7 +2416,7 @@
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="13"/>
       <c r="B152" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C152" s="21"/>
       <c r="D152" s="21"/>
@@ -2451,14 +2448,14 @@
         <v>0</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D157" s="5"/>
       <c r="E157" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F157" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G157" s="6"/>
     </row>
@@ -2477,7 +2474,7 @@
         <v>2</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D159" s="5"/>
       <c r="E159" s="10" t="s">
@@ -2511,7 +2508,7 @@
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
@@ -2522,7 +2519,7 @@
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C163" s="8"/>
       <c r="D163" s="8"/>
@@ -2553,7 +2550,7 @@
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
@@ -2564,7 +2561,7 @@
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C167" s="8"/>
       <c r="D167" s="8"/>
@@ -2584,7 +2581,7 @@
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="13"/>
       <c r="B169" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C169" s="15"/>
       <c r="D169" s="15"/>
@@ -2595,7 +2592,7 @@
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
       <c r="B170" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C170" s="18"/>
       <c r="D170" s="18"/>
@@ -2606,7 +2603,7 @@
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="13"/>
       <c r="B171" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
@@ -2617,7 +2614,7 @@
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="13"/>
       <c r="B172" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C172" s="15"/>
       <c r="D172" s="15"/>
@@ -2628,7 +2625,7 @@
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
       <c r="B173" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C173" s="15"/>
       <c r="D173" s="15"/>
@@ -2639,7 +2636,7 @@
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="13"/>
       <c r="B174" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C174" s="21"/>
       <c r="D174" s="21"/>
@@ -2671,14 +2668,14 @@
         <v>0</v>
       </c>
       <c r="C179" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D179" s="5"/>
       <c r="E179" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F179" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G179" s="6"/>
     </row>
@@ -2697,7 +2694,7 @@
         <v>2</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D181" s="5"/>
       <c r="E181" s="10" t="s">
@@ -2731,7 +2728,7 @@
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
@@ -2742,7 +2739,7 @@
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C185" s="8"/>
       <c r="D185" s="8"/>
@@ -2773,7 +2770,7 @@
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -2784,7 +2781,7 @@
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="8"/>
@@ -2804,7 +2801,7 @@
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
       <c r="B191" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
@@ -2815,7 +2812,7 @@
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="13"/>
       <c r="B192" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C192" s="18"/>
       <c r="D192" s="18"/>
@@ -2826,7 +2823,7 @@
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="13"/>
       <c r="B193" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
@@ -2837,7 +2834,7 @@
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="13"/>
       <c r="B194" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C194" s="15"/>
       <c r="D194" s="15"/>
@@ -2848,7 +2845,7 @@
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="13"/>
       <c r="B195" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C195" s="15"/>
       <c r="D195" s="15"/>
@@ -2889,14 +2886,14 @@
         <v>0</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D201" s="5"/>
       <c r="E201" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F201" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G201" s="6"/>
     </row>
@@ -2915,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="C203" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D203" s="5"/>
       <c r="E203" s="10" t="s">
@@ -2949,7 +2946,7 @@
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
@@ -2960,7 +2957,7 @@
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C207" s="8"/>
       <c r="D207" s="8"/>
@@ -2991,7 +2988,7 @@
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="1" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
@@ -3002,7 +2999,7 @@
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="8"/>
@@ -3022,7 +3019,7 @@
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="13"/>
       <c r="B213" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C213" s="15"/>
       <c r="D213" s="15"/>
@@ -3033,7 +3030,7 @@
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="13"/>
       <c r="B214" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C214" s="18"/>
       <c r="D214" s="18"/>
@@ -3044,7 +3041,7 @@
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
       <c r="B215" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C215" s="15"/>
       <c r="D215" s="15"/>
@@ -3055,7 +3052,7 @@
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="13"/>
       <c r="B216" s="13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C216" s="15"/>
       <c r="D216" s="15"/>
@@ -3066,7 +3063,7 @@
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
       <c r="B217" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C217" s="15"/>
       <c r="D217" s="15"/>
@@ -3077,7 +3074,7 @@
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="13"/>
       <c r="B218" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C218" s="21"/>
       <c r="D218" s="21"/>
@@ -3109,14 +3106,14 @@
         <v>0</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D223" s="5"/>
       <c r="E223" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F223" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G223" s="6"/>
     </row>
@@ -3129,13 +3126,13 @@
       <c r="F224" s="5"/>
       <c r="G224" s="6"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D225" s="5"/>
       <c r="E225" s="10" t="s">
@@ -3146,7 +3143,7 @@
       </c>
       <c r="G225" s="6"/>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
       <c r="C226" s="5"/>
@@ -3155,7 +3152,7 @@
       <c r="F226" s="5"/>
       <c r="G226" s="6"/>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="12" t="s">
         <v>4</v>
@@ -3166,10 +3163,10 @@
       <c r="F227" s="5"/>
       <c r="G227" s="6"/>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
@@ -3177,10 +3174,10 @@
       <c r="F228" s="3"/>
       <c r="G228" s="6"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C229" s="8"/>
       <c r="D229" s="8"/>
@@ -3188,7 +3185,7 @@
       <c r="F229" s="9"/>
       <c r="G229" s="6"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
       <c r="C230" s="5"/>
@@ -3197,7 +3194,7 @@
       <c r="F230" s="5"/>
       <c r="G230" s="6"/>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="12" t="s">
         <v>5</v>
@@ -3208,10 +3205,10 @@
       <c r="F231" s="5"/>
       <c r="G231" s="6"/>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
@@ -3219,10 +3216,10 @@
       <c r="F232" s="3"/>
       <c r="G232" s="6"/>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C233" s="8"/>
       <c r="D233" s="8"/>
@@ -3230,7 +3227,7 @@
       <c r="F233" s="9"/>
       <c r="G233" s="6"/>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
       <c r="C234" s="5"/>
@@ -3239,10 +3236,10 @@
       <c r="F234" s="5"/>
       <c r="G234" s="6"/>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" s="13"/>
       <c r="B235" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C235" s="15"/>
       <c r="D235" s="15"/>
@@ -3250,10 +3247,10 @@
       <c r="F235" s="15"/>
       <c r="G235" s="16"/>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" s="13"/>
       <c r="B236" s="17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C236" s="18"/>
       <c r="D236" s="18"/>
@@ -3261,10 +3258,10 @@
       <c r="F236" s="19"/>
       <c r="G236" s="16"/>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
       <c r="B237" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C237" s="15"/>
       <c r="D237" s="15"/>
@@ -3272,21 +3269,22 @@
       <c r="F237" s="16"/>
       <c r="G237" s="16"/>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" s="13"/>
       <c r="B238" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C238" s="15"/>
       <c r="D238" s="15"/>
       <c r="E238" s="15"/>
       <c r="F238" s="16"/>
       <c r="G238" s="16"/>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O238" s="23"/>
+    </row>
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" s="13"/>
       <c r="B239" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C239" s="15"/>
       <c r="D239" s="15"/>
@@ -3294,10 +3292,10 @@
       <c r="F239" s="16"/>
       <c r="G239" s="16"/>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
       <c r="B240" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C240" s="21"/>
       <c r="D240" s="21"/>
@@ -3305,7 +3303,7 @@
       <c r="F240" s="22"/>
       <c r="G240" s="16"/>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" s="20"/>
       <c r="B241" s="21"/>
       <c r="C241" s="21"/>
@@ -3314,7 +3312,7 @@
       <c r="F241" s="21"/>
       <c r="G241" s="22"/>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
@@ -3323,24 +3321,24 @@
       <c r="F244" s="2"/>
       <c r="G244" s="3"/>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" s="4"/>
       <c r="B245" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C245" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D245" s="5"/>
       <c r="E245" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F245" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G245" s="6"/>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" s="4"/>
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
@@ -3349,13 +3347,13 @@
       <c r="F246" s="5"/>
       <c r="G246" s="6"/>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" s="4"/>
       <c r="B247" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C247" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D247" s="5"/>
       <c r="E247" s="10" t="s">
@@ -3366,7 +3364,7 @@
       </c>
       <c r="G247" s="6"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="4"/>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
@@ -3375,7 +3373,7 @@
       <c r="F248" s="5"/>
       <c r="G248" s="6"/>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="4"/>
       <c r="B249" s="12" t="s">
         <v>4</v>
@@ -3386,10 +3384,10 @@
       <c r="F249" s="5"/>
       <c r="G249" s="6"/>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="4"/>
       <c r="B250" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
@@ -3397,10 +3395,10 @@
       <c r="F250" s="3"/>
       <c r="G250" s="6"/>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="4"/>
       <c r="B251" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C251" s="8"/>
       <c r="D251" s="8"/>
@@ -3408,7 +3406,7 @@
       <c r="F251" s="9"/>
       <c r="G251" s="6"/>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="4"/>
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
@@ -3417,7 +3415,7 @@
       <c r="F252" s="5"/>
       <c r="G252" s="6"/>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="4"/>
       <c r="B253" s="12" t="s">
         <v>5</v>
@@ -3428,10 +3426,10 @@
       <c r="F253" s="5"/>
       <c r="G253" s="6"/>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="4"/>
       <c r="B254" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
@@ -3439,18 +3437,19 @@
       <c r="F254" s="3"/>
       <c r="G254" s="6"/>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="4"/>
       <c r="B255" s="7" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C255" s="8"/>
       <c r="D255" s="8"/>
       <c r="E255" s="8"/>
       <c r="F255" s="9"/>
       <c r="G255" s="6"/>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L255" s="23"/>
+    </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="4"/>
       <c r="B256" s="5"/>
       <c r="C256" s="5"/>
@@ -3462,7 +3461,7 @@
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="13"/>
       <c r="B257" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C257" s="15"/>
       <c r="D257" s="15"/>
@@ -3473,7 +3472,7 @@
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="13"/>
       <c r="B258" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C258" s="18"/>
       <c r="D258" s="18"/>
@@ -3484,7 +3483,7 @@
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
       <c r="B259" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C259" s="15"/>
       <c r="D259" s="15"/>
@@ -3495,7 +3494,7 @@
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="13"/>
       <c r="B260" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C260" s="15"/>
       <c r="D260" s="15"/>
@@ -3506,7 +3505,7 @@
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="13"/>
       <c r="B261" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C261" s="15"/>
       <c r="D261" s="15"/>
@@ -3547,14 +3546,14 @@
         <v>0</v>
       </c>
       <c r="C267" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D267" s="5"/>
       <c r="E267" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F267" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G267" s="6"/>
     </row>
@@ -3573,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="C269" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D269" s="5"/>
       <c r="E269" s="10" t="s">
@@ -3607,7 +3606,7 @@
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="4"/>
       <c r="B272" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
@@ -3618,7 +3617,7 @@
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="4"/>
       <c r="B273" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C273" s="8"/>
       <c r="D273" s="8"/>
@@ -3649,7 +3648,7 @@
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="4"/>
       <c r="B276" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
@@ -3680,7 +3679,7 @@
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
       <c r="B279" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C279" s="15"/>
       <c r="D279" s="15"/>
@@ -3691,7 +3690,7 @@
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="13"/>
       <c r="B280" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C280" s="18"/>
       <c r="D280" s="18"/>
@@ -3702,7 +3701,7 @@
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="13"/>
       <c r="B281" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C281" s="15"/>
       <c r="D281" s="15"/>
@@ -3713,7 +3712,7 @@
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="13"/>
       <c r="B282" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C282" s="15"/>
       <c r="D282" s="15"/>
@@ -3724,7 +3723,7 @@
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="13"/>
       <c r="B283" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C283" s="15"/>
       <c r="D283" s="15"/>

</xml_diff>